<commit_message>
Test run fro dale
</commit_message>
<xml_diff>
--- a/Calc of mecanum wheel.xlsx
+++ b/Calc of mecanum wheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Mechanical_Eng\Fremantle\DALE atts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p447144\Documents\mecanum-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>V0</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">crabbing </t>
+  </si>
+  <si>
+    <t>Dale was here</t>
   </si>
 </sst>
 </file>
@@ -621,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G27"/>
+  <dimension ref="A4:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,6 +882,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F10:G10"/>

</xml_diff>

<commit_message>
Revert "Test run fro dale"
This reverts commit 1a391a3d6815b333423a455521da73a21242a7f0.
</commit_message>
<xml_diff>
--- a/Calc of mecanum wheel.xlsx
+++ b/Calc of mecanum wheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p447144\Documents\mecanum-doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Mechanical_Eng\Fremantle\DALE atts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>V0</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t xml:space="preserve">crabbing </t>
-  </si>
-  <si>
-    <t>Dale was here</t>
   </si>
 </sst>
 </file>
@@ -624,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G30"/>
+  <dimension ref="A4:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,11 +879,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F10:G10"/>

</xml_diff>

<commit_message>
Addition of tolerances document
</commit_message>
<xml_diff>
--- a/Calc of mecanum wheel.xlsx
+++ b/Calc of mecanum wheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P136265\Documents\GitHub\mecanum-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>V0</t>
   </si>
@@ -214,12 +214,30 @@
   </si>
   <si>
     <t>weight distribution (Straight) (N.m)</t>
+  </si>
+  <si>
+    <t>Keyway force</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>Keyway area</t>
+  </si>
+  <si>
+    <t>Keyway stress</t>
+  </si>
+  <si>
+    <t>Mpa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,6 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,15 +614,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:N30"/>
+  <dimension ref="A4:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="46.7109375" bestFit="1" customWidth="1"/>
@@ -660,7 +680,7 @@
         <v>27</v>
       </c>
       <c r="C7">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -680,7 +700,7 @@
       </c>
       <c r="C9">
         <f>(C7+C8)*(9.81)</f>
-        <v>6621.75</v>
+        <v>10545.75</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -692,7 +712,7 @@
       </c>
       <c r="C10">
         <f>(C7+C8)</f>
-        <v>675</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -704,7 +724,7 @@
       </c>
       <c r="C11">
         <f>C16*C18*1.15</f>
-        <v>24.847219124999999</v>
+        <v>39.571497125</v>
       </c>
       <c r="N11" t="s">
         <v>35</v>
@@ -730,7 +750,7 @@
       </c>
       <c r="C13" s="6">
         <f>C12*C9</f>
-        <v>99.326250000000002</v>
+        <v>158.18625</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -742,7 +762,7 @@
       </c>
       <c r="C14" s="6">
         <f>C10*C4</f>
-        <v>112.50000000000001</v>
+        <v>179.16666666666669</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>36</v>
@@ -767,7 +787,7 @@
       </c>
       <c r="C15" s="4">
         <f>SIN(E15)*C9</f>
-        <v>231.09574228978579</v>
+        <v>368.04136735039958</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
@@ -781,11 +801,11 @@
       </c>
       <c r="H15" s="9">
         <f>(C15+C14+C13)*C18*1.15*1.41</f>
-        <v>73.256197070784523</v>
+        <v>116.66727681643461</v>
       </c>
       <c r="I15" s="4">
         <f>H15/4</f>
-        <v>18.314049267696131</v>
+        <v>29.166819204108652</v>
       </c>
       <c r="J15" s="10">
         <v>0.6</v>
@@ -803,15 +823,15 @@
       </c>
       <c r="C16" s="6">
         <f>C13+C14</f>
-        <v>211.82625000000002</v>
+        <v>337.35291666666672</v>
       </c>
       <c r="J16" s="4">
         <f>0.6*H15</f>
-        <v>43.953718242470714</v>
+        <v>70.000366089860762</v>
       </c>
       <c r="K16" s="4">
         <f>0.4*H15</f>
-        <v>29.302478828313809</v>
+        <v>46.666910726573846</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -826,11 +846,11 @@
       </c>
       <c r="J17" s="4">
         <f>J16/2</f>
-        <v>21.976859121235357</v>
+        <v>35.000183044930381</v>
       </c>
       <c r="K17" s="4">
         <f>K16/2</f>
-        <v>14.651239414156905</v>
+        <v>23.333455363286923</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -863,7 +883,7 @@
       </c>
       <c r="E21" s="6">
         <f>C11*C21</f>
-        <v>35.034578966249995</v>
+        <v>55.79581094625</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>13</v>
@@ -881,7 +901,7 @@
       </c>
       <c r="E22" s="6">
         <f>C11*C22</f>
-        <v>31.059023906249998</v>
+        <v>49.464371406250002</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>13</v>
@@ -914,19 +934,19 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>0.6*E21</f>
-        <v>21.020747379749995</v>
+        <v>33.477486567749999</v>
       </c>
       <c r="C26">
         <f>0.4*E21</f>
-        <v>14.013831586499998</v>
+        <v>22.318324378500002</v>
       </c>
       <c r="E26">
         <f>0.6*E22</f>
-        <v>18.635414343749996</v>
+        <v>29.678622843749999</v>
       </c>
       <c r="F26">
         <f>0.4*E22</f>
-        <v>12.423609562499999</v>
+        <v>19.785748562500004</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -935,19 +955,19 @@
       </c>
       <c r="B27" s="6">
         <f>B26/2</f>
-        <v>10.510373689874998</v>
+        <v>16.738743283874999</v>
       </c>
       <c r="C27" s="6">
         <f>C26/2</f>
-        <v>7.0069157932499992</v>
+        <v>11.159162189250001</v>
       </c>
       <c r="E27" s="11">
         <f>E26/2</f>
-        <v>9.3177071718749982</v>
+        <v>14.839311421874999</v>
       </c>
       <c r="F27" s="11">
         <f>F26/2</f>
-        <v>6.2118047812499997</v>
+        <v>9.8928742812500019</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -967,6 +987,42 @@
         <f>E6/C18</f>
         <v>8.169934640522877</v>
       </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <f>B26/(20/2)</f>
+        <v>3.3477486567749999</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <f>0.02*0.0025*2</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <f>(B32)/(B33*1000)</f>
+        <v>33.477486567749999</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>